<commit_message>
changed input excel sheet
</commit_message>
<xml_diff>
--- a/engine/assets/data/KORSBAEK_EXCELTEMPLATE_v2.xlsx
+++ b/engine/assets/data/KORSBAEK_EXCELTEMPLATE_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FrederikKaae\Desktop\scheduling\engine\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14893758-F84B-40CB-9353-A6F38D71BAFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7247463-7C81-49E9-B18A-F78ACC87BBFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7680" activeTab="2" xr2:uid="{9AFE961F-F75F-4EBD-91A2-911D1E5F9EEC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="587">
   <si>
     <t>This is the mapping for the Korsbæk scene planner v0.1
 All information within this document will be used as parameters for computing a possible scene plan for a given day</t>
@@ -1513,9 +1513,6 @@
     <t>SVINSKE</t>
   </si>
   <si>
-    <t>HUSLIG</t>
-  </si>
-  <si>
     <t>SVANGERSKABSSAGER</t>
   </si>
   <si>
@@ -1787,6 +1784,21 @@
   </si>
   <si>
     <t>VELKOMMEN</t>
+  </si>
+  <si>
+    <t>NB: HUSK AT HØR FAR</t>
+  </si>
+  <si>
+    <t>HUSLIG2</t>
+  </si>
+  <si>
+    <t>Huslig værnepligt 2</t>
+  </si>
+  <si>
+    <t>Fernandos skimmel 2</t>
+  </si>
+  <si>
+    <t>Spirella 2</t>
   </si>
 </sst>
 </file>
@@ -1932,7 +1944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1960,6 +1972,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2430,7 +2443,7 @@
   <dimension ref="A1:AE13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2547,7 +2560,7 @@
         <v>225</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="AC1" s="3" t="s">
         <v>329</v>
@@ -3711,8 +3724,8 @@
   <dimension ref="A1:AM164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B165" sqref="B165"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10836,7 +10849,7 @@
         <v>335</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C62" s="27" t="s">
         <v>78</v>
@@ -11068,7 +11081,7 @@
         <v>337</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C64" s="27" t="s">
         <v>78</v>
@@ -11184,7 +11197,7 @@
         <v>338</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C65" s="27" t="s">
         <v>183</v>
@@ -11300,7 +11313,7 @@
         <v>339</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C66" s="27" t="s">
         <v>183</v>
@@ -11532,7 +11545,7 @@
         <v>341</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C68" s="27" t="s">
         <v>60</v>
@@ -11880,7 +11893,7 @@
         <v>344</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C71" s="27" t="s">
         <v>60</v>
@@ -11996,7 +12009,7 @@
         <v>345</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C72" s="27" t="s">
         <v>60</v>
@@ -12228,7 +12241,7 @@
         <v>347</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C74" s="27" t="s">
         <v>60</v>
@@ -12344,7 +12357,7 @@
         <v>348</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C75" s="27" t="s">
         <v>188</v>
@@ -12460,7 +12473,7 @@
         <v>349</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C76" s="27" t="s">
         <v>188</v>
@@ -12576,7 +12589,7 @@
         <v>350</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C77" s="27" t="s">
         <v>79</v>
@@ -12808,7 +12821,7 @@
         <v>352</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C79" s="27" t="s">
         <v>79</v>
@@ -12926,7 +12939,9 @@
       <c r="B80" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="C80" s="27"/>
+      <c r="C80" s="32" t="s">
+        <v>582</v>
+      </c>
       <c r="D80" s="27">
         <v>0</v>
       </c>
@@ -13038,9 +13053,11 @@
         <v>354</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="C81" s="27"/>
+        <v>505</v>
+      </c>
+      <c r="C81" s="27" t="s">
+        <v>582</v>
+      </c>
       <c r="D81" s="27">
         <v>0</v>
       </c>
@@ -13149,10 +13166,10 @@
     </row>
     <row r="82" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A82" s="25" t="s">
-        <v>127</v>
+        <v>584</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>491</v>
+        <v>583</v>
       </c>
       <c r="C82" s="27" t="s">
         <v>188</v>
@@ -13384,7 +13401,7 @@
         <v>356</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C84" s="27" t="s">
         <v>188</v>
@@ -13500,7 +13517,7 @@
         <v>357</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C85" s="27" t="s">
         <v>188</v>
@@ -13732,7 +13749,7 @@
         <v>359</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C87" s="27" t="s">
         <v>188</v>
@@ -13964,7 +13981,7 @@
         <v>361</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C89" s="27" t="s">
         <v>188</v>
@@ -14080,7 +14097,7 @@
         <v>362</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C90" s="27" t="s">
         <v>188</v>
@@ -14196,7 +14213,7 @@
         <v>363</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C91" s="27" t="s">
         <v>396</v>
@@ -14309,10 +14326,10 @@
     </row>
     <row r="92" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A92" s="25" t="s">
-        <v>118</v>
+        <v>585</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C92" s="27" t="s">
         <v>188</v>
@@ -14428,7 +14445,7 @@
         <v>364</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C93" s="27" t="s">
         <v>396</v>
@@ -14544,7 +14561,7 @@
         <v>365</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C94" s="27" t="s">
         <v>77</v>
@@ -14660,7 +14677,7 @@
         <v>366</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C95" s="27" t="s">
         <v>76</v>
@@ -14776,7 +14793,7 @@
         <v>367</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C96" s="27" t="s">
         <v>77</v>
@@ -14892,7 +14909,7 @@
         <v>368</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C97" s="27" t="s">
         <v>79</v>
@@ -15008,7 +15025,7 @@
         <v>369</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C98" s="27" t="s">
         <v>77</v>
@@ -15124,7 +15141,7 @@
         <v>370</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C99" s="27" t="s">
         <v>77</v>
@@ -15240,7 +15257,7 @@
         <v>371</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C100" s="27" t="s">
         <v>395</v>
@@ -15356,7 +15373,7 @@
         <v>372</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C101" s="27" t="s">
         <v>395</v>
@@ -15472,7 +15489,7 @@
         <v>373</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C102" s="27" t="s">
         <v>79</v>
@@ -15588,7 +15605,7 @@
         <v>397</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C103" s="30" t="s">
         <v>74</v>
@@ -15707,7 +15724,7 @@
         <v>398</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C104" s="30" t="s">
         <v>79</v>
@@ -15824,7 +15841,7 @@
         <v>399</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C105" s="30" t="s">
         <v>74</v>
@@ -15943,7 +15960,7 @@
         <v>400</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C106" s="30" t="s">
         <v>78</v>
@@ -16060,7 +16077,7 @@
         <v>401</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C107" s="30" t="s">
         <v>183</v>
@@ -16177,7 +16194,7 @@
         <v>402</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C108" s="30" t="s">
         <v>79</v>
@@ -16294,7 +16311,7 @@
         <v>403</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C109" s="30" t="s">
         <v>79</v>
@@ -16411,7 +16428,7 @@
         <v>404</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C110" s="30" t="s">
         <v>79</v>
@@ -16528,7 +16545,7 @@
         <v>405</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C111" s="30" t="s">
         <v>79</v>
@@ -16645,7 +16662,7 @@
         <v>406</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C112" s="30" t="s">
         <v>467</v>
@@ -16759,10 +16776,10 @@
     </row>
     <row r="113" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A113" s="28" t="s">
-        <v>172</v>
+        <v>586</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C113" s="30" t="s">
         <v>468</v>
@@ -16879,7 +16896,7 @@
         <v>407</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C114" s="30" t="s">
         <v>188</v>
@@ -16996,7 +17013,7 @@
         <v>408</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C115" s="30" t="s">
         <v>79</v>
@@ -17113,7 +17130,7 @@
         <v>409</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C116" s="30" t="s">
         <v>79</v>
@@ -17230,7 +17247,7 @@
         <v>410</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C117" s="30" t="s">
         <v>469</v>
@@ -17347,7 +17364,7 @@
         <v>411</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C118" s="30" t="s">
         <v>76</v>
@@ -17466,7 +17483,7 @@
         <v>412</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C119" s="30" t="s">
         <v>60</v>
@@ -17585,7 +17602,7 @@
         <v>413</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C120" s="30" t="s">
         <v>78</v>
@@ -17702,7 +17719,7 @@
         <v>414</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C121" s="30" t="s">
         <v>188</v>
@@ -17819,7 +17836,7 @@
         <v>415</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C122" s="30" t="s">
         <v>79</v>
@@ -17936,7 +17953,7 @@
         <v>416</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C123" s="30" t="s">
         <v>79</v>
@@ -18053,7 +18070,7 @@
         <v>417</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C124" s="30" t="s">
         <v>79</v>
@@ -18169,7 +18186,7 @@
         <v>418</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C125" s="30" t="s">
         <v>188</v>
@@ -18285,7 +18302,7 @@
         <v>419</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C126" s="30" t="s">
         <v>186</v>
@@ -18401,7 +18418,7 @@
         <v>420</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C127" s="30" t="s">
         <v>77</v>
@@ -18517,7 +18534,7 @@
         <v>421</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C128" s="30" t="s">
         <v>186</v>
@@ -18633,7 +18650,7 @@
         <v>422</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C129" s="30" t="s">
         <v>188</v>
@@ -18749,7 +18766,7 @@
         <v>423</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C130" s="30" t="s">
         <v>79</v>
@@ -18865,7 +18882,7 @@
         <v>424</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C131" s="30" t="s">
         <v>79</v>
@@ -18981,7 +18998,7 @@
         <v>425</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C132" s="30" t="s">
         <v>188</v>
@@ -19097,7 +19114,7 @@
         <v>426</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C133" s="30" t="s">
         <v>469</v>
@@ -19329,7 +19346,7 @@
         <v>428</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C135" s="30" t="s">
         <v>77</v>
@@ -19445,7 +19462,7 @@
         <v>429</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C136" s="30" t="s">
         <v>468</v>
@@ -19561,7 +19578,7 @@
         <v>430</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C137" s="30" t="s">
         <v>468</v>
@@ -19677,7 +19694,7 @@
         <v>431</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C138" s="30" t="s">
         <v>78</v>
@@ -19793,7 +19810,7 @@
         <v>432</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C139" s="30" t="s">
         <v>468</v>
@@ -19909,7 +19926,7 @@
         <v>433</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C140" s="30" t="s">
         <v>79</v>
@@ -20026,7 +20043,7 @@
         <v>434</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C141" s="30" t="s">
         <v>79</v>
@@ -20143,7 +20160,7 @@
         <v>435</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C142" s="30" t="s">
         <v>470</v>
@@ -20260,7 +20277,7 @@
         <v>436</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C143" s="30" t="s">
         <v>186</v>
@@ -20377,7 +20394,7 @@
         <v>437</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C144" s="30" t="s">
         <v>76</v>
@@ -20496,7 +20513,7 @@
         <v>438</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C145" s="30" t="s">
         <v>79</v>
@@ -20613,7 +20630,7 @@
         <v>439</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C146" s="30" t="s">
         <v>79</v>
@@ -20730,7 +20747,7 @@
         <v>440</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C147" s="30" t="s">
         <v>471</v>
@@ -20847,7 +20864,7 @@
         <v>441</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C148" s="30" t="s">
         <v>468</v>
@@ -20964,7 +20981,7 @@
         <v>442</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C149" s="30" t="s">
         <v>79</v>
@@ -21081,7 +21098,7 @@
         <v>443</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C150" s="30" t="s">
         <v>188</v>
@@ -21198,7 +21215,7 @@
         <v>444</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C151" s="30" t="s">
         <v>188</v>
@@ -21315,7 +21332,7 @@
         <v>445</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C152" s="30" t="s">
         <v>79</v>
@@ -21432,7 +21449,7 @@
         <v>446</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C153" s="30" t="s">
         <v>186</v>
@@ -21549,7 +21566,7 @@
         <v>447</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C154" s="30" t="s">
         <v>472</v>
@@ -21666,7 +21683,7 @@
         <v>448</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C155" s="30" t="s">
         <v>468</v>
@@ -21783,7 +21800,7 @@
         <v>449</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C156" s="30" t="s">
         <v>79</v>
@@ -21900,7 +21917,7 @@
         <v>450</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C157" s="30" t="s">
         <v>78</v>
@@ -22019,7 +22036,7 @@
         <v>451</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C158" s="30" t="s">
         <v>469</v>
@@ -22136,7 +22153,7 @@
         <v>452</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C159" s="30" t="s">
         <v>468</v>
@@ -22253,7 +22270,7 @@
         <v>453</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C160" s="30" t="s">
         <v>76</v>
@@ -22370,7 +22387,7 @@
         <v>454</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C161" s="30" t="s">
         <v>473</v>
@@ -22487,7 +22504,7 @@
         <v>455</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C162" s="30" t="s">
         <v>79</v>
@@ -22604,7 +22621,7 @@
         <v>456</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C163" s="30" t="s">
         <v>468</v>
@@ -22721,7 +22738,7 @@
         <v>457</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C164" s="30" t="s">
         <v>78</v>

</xml_diff>